<commit_message>
Export Excel Command v1.3
</commit_message>
<xml_diff>
--- a/Financial_Planner_31-03-1999_31-3-2018.xlsx
+++ b/Financial_Planner_31-03-1999_31-3-2018.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NAME</t>
   </si>
@@ -23,22 +23,10 @@
     <t>MONEY SPENT/RECEIVED</t>
   </si>
   <si>
-    <t>Charlotte Oliveiro</t>
+    <t>Payment for Caifan</t>
   </si>
   <si>
-    <t>29-5-1999</t>
-  </si>
-  <si>
-    <t>David Li</t>
-  </si>
-  <si>
-    <t>30-6-2014</t>
-  </si>
-  <si>
-    <t>Roy Balakrishnan</t>
-  </si>
-  <si>
-    <t>15-7-2005</t>
+    <t>18-2-2018</t>
   </si>
 </sst>
 </file>
@@ -83,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,29 +96,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>24.49</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-437.49</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>24.5</v>
+        <v>73.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>